<commit_message>
Played with making go a little faster
</commit_message>
<xml_diff>
--- a/201309_RomanNumerals/RomanNumeralsTimeResults.xlsx
+++ b/201309_RomanNumerals/RomanNumeralsTimeResults.xlsx
@@ -391,7 +391,7 @@
         </is>
       </c>
       <c r="E2">
-        <v>3363</v>
+        <v>3507</v>
       </c>
     </row>
     <row r="3">
@@ -412,7 +412,7 @@
         </is>
       </c>
       <c r="E3">
-        <v>585</v>
+        <v>606</v>
       </c>
     </row>
     <row r="4">
@@ -433,7 +433,7 @@
         </is>
       </c>
       <c r="E4">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="5">
@@ -454,7 +454,7 @@
         </is>
       </c>
       <c r="E5">
-        <v>3047</v>
+        <v>3034</v>
       </c>
     </row>
     <row r="6">
@@ -475,7 +475,7 @@
         </is>
       </c>
       <c r="E6">
-        <v>4511</v>
+        <v>4485</v>
       </c>
     </row>
     <row r="7">
@@ -496,7 +496,7 @@
         </is>
       </c>
       <c r="E7">
-        <v>3161</v>
+        <v>3488</v>
       </c>
     </row>
     <row r="8">
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="E8">
-        <v>10473</v>
+        <v>10304</v>
       </c>
     </row>
     <row r="9">
@@ -538,7 +538,7 @@
         </is>
       </c>
       <c r="E9">
-        <v>14707</v>
+        <v>14669</v>
       </c>
     </row>
     <row r="10">
@@ -559,7 +559,7 @@
         </is>
       </c>
       <c r="E10">
-        <v>2375</v>
+        <v>2397</v>
       </c>
     </row>
     <row r="11">
@@ -580,7 +580,7 @@
         </is>
       </c>
       <c r="E11">
-        <v>6437</v>
+        <v>6528</v>
       </c>
     </row>
     <row r="12">
@@ -601,7 +601,7 @@
         </is>
       </c>
       <c r="E12">
-        <v>2936</v>
+        <v>3064</v>
       </c>
     </row>
     <row r="13">
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="E13">
-        <v>5606</v>
+        <v>8665</v>
       </c>
     </row>
     <row r="14">
@@ -643,7 +643,7 @@
         </is>
       </c>
       <c r="E14">
-        <v>4575</v>
+        <v>4663</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a clojure example to the RomanNumerals section for references. I mosly 'borrowed' this from the web but had to modify it a little to get to work correctly.
</commit_message>
<xml_diff>
--- a/201309_RomanNumerals/RomanNumeralsTimeResults.xlsx
+++ b/201309_RomanNumerals/RomanNumeralsTimeResults.xlsx
@@ -391,7 +391,7 @@
         </is>
       </c>
       <c r="E2">
-        <v>3507</v>
+        <v>3483</v>
       </c>
     </row>
     <row r="3">
@@ -412,7 +412,7 @@
         </is>
       </c>
       <c r="E3">
-        <v>606</v>
+        <v>582</v>
       </c>
     </row>
     <row r="4">
@@ -454,7 +454,7 @@
         </is>
       </c>
       <c r="E5">
-        <v>3034</v>
+        <v>2998</v>
       </c>
     </row>
     <row r="6">
@@ -475,7 +475,7 @@
         </is>
       </c>
       <c r="E6">
-        <v>4485</v>
+        <v>4530</v>
       </c>
     </row>
     <row r="7">
@@ -496,7 +496,7 @@
         </is>
       </c>
       <c r="E7">
-        <v>3488</v>
+        <v>3387</v>
       </c>
     </row>
     <row r="8">
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="E8">
-        <v>10304</v>
+        <v>10389</v>
       </c>
     </row>
     <row r="9">
@@ -538,7 +538,7 @@
         </is>
       </c>
       <c r="E9">
-        <v>14669</v>
+        <v>15014</v>
       </c>
     </row>
     <row r="10">
@@ -559,7 +559,7 @@
         </is>
       </c>
       <c r="E10">
-        <v>2397</v>
+        <v>2334</v>
       </c>
     </row>
     <row r="11">
@@ -580,7 +580,7 @@
         </is>
       </c>
       <c r="E11">
-        <v>6528</v>
+        <v>6497</v>
       </c>
     </row>
     <row r="12">
@@ -601,7 +601,7 @@
         </is>
       </c>
       <c r="E12">
-        <v>3064</v>
+        <v>3219</v>
       </c>
     </row>
     <row r="13">
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="E13">
-        <v>8665</v>
+        <v>8841</v>
       </c>
     </row>
     <row r="14">
@@ -643,7 +643,7 @@
         </is>
       </c>
       <c r="E14">
-        <v>4663</v>
+        <v>4528</v>
       </c>
     </row>
   </sheetData>

</xml_diff>